<commit_message>
Added messages boxes to notifiy user of the progress of the automation
</commit_message>
<xml_diff>
--- a/Collate hour worked from employees ReFramework/Database/Employee_payroll_table_07_09_2020.xlsx
+++ b/Collate hour worked from employees ReFramework/Database/Employee_payroll_table_07_09_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\HR automation\automation\HR-Payroll-automation\Collate hour worked from employees ReFramework\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515B1187-140B-4182-B2FD-5450EF69420C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D874B780-B1E3-46B3-BB9E-DCE2758518B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25440" yWindow="5175" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,6 +110,21 @@
     <t>Logistics</t>
   </si>
   <si>
+    <t>Maryann</t>
+  </si>
+  <si>
+    <t>Randall</t>
+  </si>
+  <si>
+    <t>cyberdynesystemsmodel545+Maryann.Randall@gmail.com</t>
+  </si>
+  <si>
+    <t>(815) 962-1403</t>
+  </si>
+  <si>
+    <t>5714 N Blackwood Rd, Davis Junction, Illinois(IL), 61020</t>
+  </si>
+  <si>
     <t>Tech</t>
   </si>
   <si>
@@ -366,21 +381,6 @@
   </si>
   <si>
     <t>15542 Jaeger Dr, Mecosta, Michigan(MI), 49332</t>
-  </si>
-  <si>
-    <t>Maryann</t>
-  </si>
-  <si>
-    <t>Randall</t>
-  </si>
-  <si>
-    <t>cyberdynesystemsmodel545+Maryann.Randall@gmail.com</t>
-  </si>
-  <si>
-    <t>(815) 962-1403</t>
-  </si>
-  <si>
-    <t>5714 N Blackwood Rd, Davis Junction, Illinois(IL), 61020</t>
   </si>
 </sst>
 </file>
@@ -802,7 +802,7 @@
         <v>18</v>
       </c>
       <c r="H2">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>80</v>
@@ -817,8 +817,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <f>H2*I2</f>
-        <v>1520</v>
+        <v>960</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -844,23 +843,23 @@
         <v>24</v>
       </c>
       <c r="H3">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I3">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="J3">
         <v>80</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
         <f>H3*I3</f>
-        <v>1440</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -868,25 +867,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4">
         <v>80</v>
@@ -901,8 +900,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f>H4*I4</f>
-        <v>1280</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -910,25 +908,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
       </c>
       <c r="H5">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I5">
         <v>80</v>
@@ -943,8 +941,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <f>H5*I5</f>
-        <v>1760</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -952,25 +949,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>
       </c>
       <c r="H6">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I6">
         <v>80</v>
@@ -985,8 +982,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <f>H6*I6</f>
-        <v>720</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -994,25 +990,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H7">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I7">
         <v>80</v>
@@ -1027,8 +1023,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <f>H7*I7</f>
-        <v>2000</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1036,25 +1031,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
       </c>
       <c r="H8">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I8">
         <v>80</v>
@@ -1069,8 +1064,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <f>H8*I8</f>
-        <v>1200</v>
+        <v>640</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1078,25 +1072,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
       </c>
       <c r="H9">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I9">
         <v>80</v>
@@ -1111,8 +1105,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <f>H9*I9</f>
-        <v>1360</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1120,25 +1113,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H10">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I10">
         <v>80</v>
@@ -1153,8 +1146,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <f>H10*I10</f>
-        <v>880</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1162,19 +1154,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
         <v>18</v>
@@ -1195,7 +1187,6 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <f>H11*I11</f>
         <v>800</v>
       </c>
     </row>
@@ -1204,25 +1195,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
       </c>
       <c r="H12">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I12">
         <v>80</v>
@@ -1237,8 +1228,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <f>H12*I12</f>
-        <v>560</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1246,25 +1236,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H13">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I13">
         <v>80</v>
@@ -1279,8 +1269,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <f>H13*I13</f>
-        <v>1440</v>
+        <v>960</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1288,25 +1277,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>
       </c>
       <c r="H14">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I14">
         <v>80</v>
@@ -1321,8 +1310,7 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <f>H14*I14</f>
-        <v>1600</v>
+        <v>960</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1330,25 +1318,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
       </c>
       <c r="H15">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I15">
         <v>80</v>
@@ -1363,8 +1351,7 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <f>H15*I15</f>
-        <v>1520</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1372,25 +1359,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H16">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I16">
         <v>80</v>
@@ -1405,8 +1392,7 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <f>H16*I16</f>
-        <v>1040</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1414,25 +1400,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="G17" t="s">
         <v>18</v>
       </c>
       <c r="H17">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I17">
         <v>80</v>
@@ -1447,8 +1433,7 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <f>H17*I17</f>
-        <v>880</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1456,25 +1441,25 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
         <v>24</v>
       </c>
       <c r="H18">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I18">
         <v>80</v>
@@ -1489,8 +1474,7 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <f>H18*I18</f>
-        <v>1440</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1498,25 +1482,25 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G19" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H19">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="I19">
         <v>80</v>
@@ -1531,8 +1515,7 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <f>H19*I19</f>
-        <v>1840</v>
+        <v>800</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1540,25 +1523,25 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F20" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
         <v>18</v>
       </c>
       <c r="H20">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I20">
         <v>80</v>
@@ -1573,8 +1556,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <f>H20*I20</f>
-        <v>1920</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1582,25 +1564,25 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E21" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F21" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G21" t="s">
         <v>24</v>
       </c>
       <c r="H21">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="I21">
         <v>80</v>
@@ -1615,8 +1597,7 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <f>H21*I21</f>
-        <v>1840</v>
+        <v>1120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>